<commit_message>
Acabada presentacion y modificado presupuesto
</commit_message>
<xml_diff>
--- a/fol/UBALDE_Presupuesto.xlsx
+++ b/fol/UBALDE_Presupuesto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grado\2e\Trabajo FCT\UBALDE_Trabajo FCT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Downloads\2h\fol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36716A77-3FFB-4A8E-B6F8-90F6C0B85BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3653E5-7B48-4631-B64E-A15CAE246773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos humanos" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="xctoebpc5000_1" localSheetId="0">'Recursos humanos'!$C$16:$C$345</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>CPD</t>
   </si>
@@ -324,9 +328,6 @@
     <t>R,T</t>
   </si>
   <si>
-    <t>R,C,CAP</t>
-  </si>
-  <si>
     <t>R,CAP</t>
   </si>
   <si>
@@ -351,9 +352,6 @@
     <t>Días estancias</t>
   </si>
   <si>
-    <t>TOTAL de todo</t>
-  </si>
-  <si>
     <t>Sin el coste de equipamiento porque no se sabe cuanto tiempo se va a necesitar</t>
   </si>
   <si>
@@ -364,6 +362,9 @@
   </si>
   <si>
     <t>Técnicos teleco</t>
+  </si>
+  <si>
+    <t>R,CA,CAP</t>
   </si>
 </sst>
 </file>
@@ -1166,6 +1167,117 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1202,33 +1314,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1238,98 +1323,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1366,54 +1415,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1471,7 +1472,7 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1800,550 +1801,550 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD261A9-C307-498A-9ABC-0594443A472D}">
   <dimension ref="A1:BD256"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL7" sqref="AL7:AO7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AL10" sqref="AL10:AO10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="38" width="3.42578125" customWidth="1"/>
-    <col min="39" max="43" width="3.5703125" customWidth="1"/>
-    <col min="44" max="44" width="3.7109375" customWidth="1"/>
-    <col min="45" max="45" width="3.28515625" customWidth="1"/>
-    <col min="46" max="47" width="3.5703125" customWidth="1"/>
-    <col min="48" max="48" width="3.42578125" customWidth="1"/>
-    <col min="49" max="49" width="3.28515625" customWidth="1"/>
-    <col min="50" max="55" width="3.42578125" customWidth="1"/>
-    <col min="56" max="56" width="3.140625" customWidth="1"/>
-    <col min="57" max="60" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="5" width="3.88671875" customWidth="1"/>
+    <col min="6" max="38" width="3.44140625" customWidth="1"/>
+    <col min="39" max="43" width="3.5546875" customWidth="1"/>
+    <col min="44" max="44" width="3.6640625" customWidth="1"/>
+    <col min="45" max="45" width="3.33203125" customWidth="1"/>
+    <col min="46" max="47" width="3.5546875" customWidth="1"/>
+    <col min="48" max="48" width="3.44140625" customWidth="1"/>
+    <col min="49" max="49" width="3.33203125" customWidth="1"/>
+    <col min="50" max="55" width="3.44140625" customWidth="1"/>
+    <col min="56" max="56" width="3.109375" customWidth="1"/>
+    <col min="57" max="60" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="36"/>
     </row>
-    <row r="5" spans="1:55" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="90" t="s">
+    <row r="5" spans="1:55" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="G5" s="52" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="G5" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="87" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="52" t="s">
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="52" t="s">
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="S5" s="53"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="71" t="s">
+      <c r="S5" s="49"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="V5" s="72"/>
-      <c r="W5" s="73"/>
-      <c r="AI5" s="71" t="s">
+      <c r="V5" s="75"/>
+      <c r="W5" s="76"/>
+      <c r="AI5" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="76"/>
+      <c r="AL5" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="50"/>
+      <c r="AP5" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AJ5" s="72"/>
-      <c r="AK5" s="73"/>
-      <c r="AL5" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM5" s="53"/>
-      <c r="AN5" s="53"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ5" s="53"/>
-      <c r="AR5" s="53"/>
-      <c r="AS5" s="54"/>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="91">
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="50"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B6" s="42">
         <v>43930</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="G6" s="85" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="G6" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="85">
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="54">
         <v>2</v>
       </c>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="80">
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="51">
         <v>43922</v>
       </c>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="80">
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="51">
         <f t="shared" ref="R6:R11" si="0">WORKDAY(O6-1,L6,$B$6:$E$15)</f>
         <v>43923</v>
       </c>
-      <c r="S6" s="81"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="55" t="s">
+      <c r="S6" s="52"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="V6" s="56"/>
-      <c r="W6" s="57"/>
-      <c r="AC6" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD6" s="56"/>
-      <c r="AE6" s="56"/>
-      <c r="AF6" s="56"/>
-      <c r="AG6" s="56"/>
-      <c r="AH6" s="57"/>
-      <c r="AI6" s="55">
+      <c r="V6" s="66"/>
+      <c r="W6" s="67"/>
+      <c r="AC6" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD6" s="66"/>
+      <c r="AE6" s="66"/>
+      <c r="AF6" s="66"/>
+      <c r="AG6" s="66"/>
+      <c r="AH6" s="67"/>
+      <c r="AI6" s="65">
         <v>3</v>
       </c>
-      <c r="AJ6" s="56"/>
-      <c r="AK6" s="57"/>
-      <c r="AL6" s="64">
+      <c r="AJ6" s="66"/>
+      <c r="AK6" s="67"/>
+      <c r="AL6" s="61">
         <f>SUM(IF(COUNTIF($U$6,"*R*"),(AI6*Subcontrataciones!D7)*$L$6,0),IF(COUNTIF($U$7,"*R*"),(AI6*Subcontrataciones!D7)*$L$7,0),IF(COUNTIF($U$8,"*R*"),(AI6*Subcontrataciones!D7)*$L$8,0),IF(COUNTIF($U$9,"*R*"),(AI6*Subcontrataciones!D7)*$L$9,0),IF(COUNTIF($U$10,"*R*"),(AI6*Subcontrataciones!D7)*$L$10,0),IF(COUNTIF($U$11,"*R*"),(AI6*Subcontrataciones!D7)*$L$11,0))*8</f>
         <v>21216</v>
       </c>
-      <c r="AM6" s="65"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="66"/>
-      <c r="AP6" s="55">
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="62"/>
+      <c r="AO6" s="63"/>
+      <c r="AP6" s="65">
         <f>R10-O6</f>
         <v>50</v>
       </c>
-      <c r="AQ6" s="56"/>
-      <c r="AR6" s="56"/>
-      <c r="AS6" s="57"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B7" s="91">
+      <c r="AQ6" s="66"/>
+      <c r="AR6" s="66"/>
+      <c r="AS6" s="67"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B7" s="42">
         <v>43931</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="G7" s="85" t="s">
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="G7" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="85">
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="54">
         <v>14</v>
       </c>
-      <c r="M7" s="86"/>
-      <c r="N7" s="86"/>
-      <c r="O7" s="80">
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="51">
         <f>R6+1</f>
         <v>43924</v>
       </c>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="80">
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="51">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="S7" s="81"/>
-      <c r="T7" s="82"/>
-      <c r="U7" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="V7" s="59"/>
-      <c r="W7" s="60"/>
-      <c r="AC7" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD7" s="59"/>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="59"/>
-      <c r="AG7" s="59"/>
-      <c r="AH7" s="60"/>
-      <c r="AI7" s="58">
+      <c r="S7" s="52"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="V7" s="69"/>
+      <c r="W7" s="70"/>
+      <c r="AC7" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
+      <c r="AH7" s="70"/>
+      <c r="AI7" s="68">
         <v>3</v>
       </c>
-      <c r="AJ7" s="59"/>
-      <c r="AK7" s="60"/>
-      <c r="AL7" s="64">
-        <f>SUM(IF(COUNTIF($U$6,"*R*"),(AI7*Subcontrataciones!D8)*$L$6,0),IF(COUNTIF($U$7,"*R*"),(AI7*Subcontrataciones!D8)*$L$7,0),IF(COUNTIF($U$8,"*R*"),(AI7*Subcontrataciones!D8)*$L$8,0),IF(COUNTIF($U$9,"*R*"),(AI7*Subcontrataciones!D8)*$L$9,0),IF(COUNTIF($U$10,"*R*"),(AI7*Subcontrataciones!D8)*$L$10,0),IF(COUNTIF($U$11,"*R*"),(AI7*Subcontrataciones!D8)*$L$11,0))*8</f>
-        <v>26112</v>
-      </c>
-      <c r="AM7" s="65"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="66"/>
-      <c r="AP7" s="58">
+      <c r="AJ7" s="69"/>
+      <c r="AK7" s="70"/>
+      <c r="AL7" s="61">
+        <f>SUM(IF(COUNTIF($U$6,"*CA*"),(AI7*Subcontrataciones!D8)*$L$6,0),IF(COUNTIF($U$7,"*CA*"),(AI7*Subcontrataciones!D8)*$L$7,0),IF(COUNTIF($U$8,"*CA*"),(AI7*Subcontrataciones!D8)*$L$8,0),IF(COUNTIF($U$9,"*CA*"),(AI7*Subcontrataciones!D8)*$L$9,0),IF(COUNTIF($U$10,"*CA*"),(AI7*Subcontrataciones!D8)*$L$10,0),IF(COUNTIF($U$11,"*CA*"),(AI7*Subcontrataciones!D8)*$L$11,0))*8</f>
+        <v>24576</v>
+      </c>
+      <c r="AM7" s="62"/>
+      <c r="AN7" s="62"/>
+      <c r="AO7" s="63"/>
+      <c r="AP7" s="68">
         <f>R8-O7</f>
         <v>33</v>
       </c>
-      <c r="AQ7" s="59"/>
-      <c r="AR7" s="59"/>
-      <c r="AS7" s="60"/>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B8" s="91">
+      <c r="AQ7" s="69"/>
+      <c r="AR7" s="69"/>
+      <c r="AS7" s="70"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B8" s="42">
         <v>43934</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="G8" s="85" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="G8" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="85">
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="54">
         <v>7</v>
       </c>
-      <c r="M8" s="86"/>
-      <c r="N8" s="86"/>
-      <c r="O8" s="80">
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="51">
         <f>R7+1</f>
         <v>43949</v>
       </c>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="80">
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="51">
         <f t="shared" si="0"/>
         <v>43957</v>
       </c>
-      <c r="S8" s="81"/>
-      <c r="T8" s="82"/>
-      <c r="U8" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="V8" s="59"/>
-      <c r="W8" s="60"/>
-      <c r="AC8" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD8" s="59"/>
-      <c r="AE8" s="59"/>
-      <c r="AF8" s="59"/>
-      <c r="AG8" s="59"/>
-      <c r="AH8" s="60"/>
-      <c r="AI8" s="58">
+      <c r="S8" s="52"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="V8" s="69"/>
+      <c r="W8" s="70"/>
+      <c r="AC8" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD8" s="69"/>
+      <c r="AE8" s="69"/>
+      <c r="AF8" s="69"/>
+      <c r="AG8" s="69"/>
+      <c r="AH8" s="70"/>
+      <c r="AI8" s="68">
         <v>2</v>
       </c>
-      <c r="AJ8" s="59"/>
-      <c r="AK8" s="60"/>
-      <c r="AL8" s="64">
-        <f>SUM(IF(COUNTIF($U$6,"*R*"),(AI8*Subcontrataciones!D9)*$L$6,0),IF(COUNTIF($U$7,"*R*"),(AI8*Subcontrataciones!D9)*$L$7,0),IF(COUNTIF($U$8,"*R*"),(AI8*Subcontrataciones!D9)*$L$8,0),IF(COUNTIF($U$9,"*R*"),(AI8*Subcontrataciones!D9)*$L$9,0),IF(COUNTIF($U$10,"*R*"),(AI8*Subcontrataciones!D9)*$L$10,0),IF(COUNTIF($U$11,"*R*"),(AI8*Subcontrataciones!D9)*$L$11,0))*8</f>
-        <v>15232</v>
-      </c>
-      <c r="AM8" s="65"/>
-      <c r="AN8" s="65"/>
-      <c r="AO8" s="66"/>
-      <c r="AP8" s="58">
+      <c r="AJ8" s="69"/>
+      <c r="AK8" s="70"/>
+      <c r="AL8" s="61">
+        <f>SUM(IF(COUNTIF($U$6,"*T*"),(AI8*Subcontrataciones!D9)*$L$6,0),IF(COUNTIF($U$7,"*T*"),(AI8*Subcontrataciones!D9)*$L$7,0),IF(COUNTIF($U$8,"*T*"),(AI8*Subcontrataciones!D9)*$L$8,0),IF(COUNTIF($U$9,"*T*"),(AI8*Subcontrataciones!D9)*$L$9,0),IF(COUNTIF($U$10,"*T*"),(AI8*Subcontrataciones!D9)*$L$10,0),IF(COUNTIF($U$11,"*T*"),(AI8*Subcontrataciones!D9)*$L$11,0))*8</f>
+        <v>3584</v>
+      </c>
+      <c r="AM8" s="62"/>
+      <c r="AN8" s="62"/>
+      <c r="AO8" s="63"/>
+      <c r="AP8" s="68">
         <v>8</v>
       </c>
-      <c r="AQ8" s="59"/>
-      <c r="AR8" s="59"/>
-      <c r="AS8" s="60"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B9" s="92">
+      <c r="AQ8" s="69"/>
+      <c r="AR8" s="69"/>
+      <c r="AS8" s="70"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B9" s="43">
         <v>43974</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
-      <c r="G9" s="85" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
+      <c r="G9" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="85">
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="54">
         <v>7</v>
       </c>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="80">
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="51">
         <f>R8+1</f>
         <v>43958</v>
       </c>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="80">
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="51">
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
-      <c r="S9" s="81"/>
-      <c r="T9" s="82"/>
-      <c r="U9" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="V9" s="59"/>
-      <c r="W9" s="60"/>
-      <c r="AC9" s="74" t="s">
+      <c r="S9" s="52"/>
+      <c r="T9" s="53"/>
+      <c r="U9" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="V9" s="69"/>
+      <c r="W9" s="70"/>
+      <c r="AC9" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="AD9" s="75"/>
-      <c r="AE9" s="75"/>
-      <c r="AF9" s="75"/>
-      <c r="AG9" s="75"/>
-      <c r="AH9" s="76"/>
-      <c r="AI9" s="58">
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="72"/>
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="72"/>
+      <c r="AH9" s="73"/>
+      <c r="AI9" s="68">
         <v>1</v>
       </c>
-      <c r="AJ9" s="59"/>
-      <c r="AK9" s="60"/>
-      <c r="AL9" s="64">
-        <f>SUM(IF(COUNTIF($U$6,"*R*"),(AI9*Subcontrataciones!D10)*$L$6,0),IF(COUNTIF($U$7,"*R*"),(AI9*Subcontrataciones!D10)*$L$7,0),IF(COUNTIF($U$8,"*R*"),(AI9*Subcontrataciones!D10)*$L$8,0),IF(COUNTIF($U$9,"*R*"),(AI9*Subcontrataciones!D10)*$L$9,0),IF(COUNTIF($U$10,"*R*"),(AI9*Subcontrataciones!D10)*$L$10,0),IF(COUNTIF($U$11,"*R*"),(AI9*Subcontrataciones!D10)*$L$11,0))*8</f>
-        <v>6256</v>
-      </c>
-      <c r="AM9" s="65"/>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="66"/>
-      <c r="AP9" s="58">
+      <c r="AJ9" s="69"/>
+      <c r="AK9" s="70"/>
+      <c r="AL9" s="61">
+        <f>SUM(IF(COUNTIF($U$6,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$6,0),IF(COUNTIF($U$7,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$7,0),IF(COUNTIF($U$8,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$8,0),IF(COUNTIF($U$9,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$9,0),IF(COUNTIF($U$10,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$10,0),IF(COUNTIF($U$11,"*CAP*"),(AI9*Subcontrataciones!D10)*$L$11,0))*8</f>
+        <v>5888</v>
+      </c>
+      <c r="AM9" s="62"/>
+      <c r="AN9" s="62"/>
+      <c r="AO9" s="63"/>
+      <c r="AP9" s="68">
         <f>R10-O7</f>
         <v>48</v>
       </c>
-      <c r="AQ9" s="59"/>
-      <c r="AR9" s="59"/>
-      <c r="AS9" s="60"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="94"/>
-      <c r="G10" s="85" t="s">
+      <c r="AQ9" s="69"/>
+      <c r="AR9" s="69"/>
+      <c r="AS9" s="70"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
+      <c r="G10" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="85">
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="54">
         <v>4</v>
       </c>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="80">
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="51">
         <f>R9+1</f>
         <v>43967</v>
       </c>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="80">
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="51">
         <f t="shared" si="0"/>
         <v>43972</v>
       </c>
-      <c r="S10" s="81"/>
-      <c r="T10" s="82"/>
-      <c r="U10" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="V10" s="59"/>
-      <c r="W10" s="60"/>
-      <c r="AI10" s="70" t="s">
+      <c r="S10" s="52"/>
+      <c r="T10" s="53"/>
+      <c r="U10" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="V10" s="69"/>
+      <c r="W10" s="70"/>
+      <c r="AI10" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="AJ10" s="70"/>
-      <c r="AK10" s="70"/>
-      <c r="AL10" s="68">
+      <c r="AJ10" s="94"/>
+      <c r="AK10" s="94"/>
+      <c r="AL10" s="93">
         <f>SUM(AL6:AO9)</f>
-        <v>68816</v>
-      </c>
-      <c r="AM10" s="69"/>
-      <c r="AN10" s="69"/>
-      <c r="AO10" s="69"/>
-      <c r="AP10" s="61">
+        <v>55264</v>
+      </c>
+      <c r="AM10" s="40"/>
+      <c r="AN10" s="40"/>
+      <c r="AO10" s="40"/>
+      <c r="AP10" s="89">
         <f>'Costes Indirectos'!D8*SUM(AP6:AS9)</f>
         <v>6255</v>
       </c>
-      <c r="AQ10" s="62"/>
-      <c r="AR10" s="62"/>
-      <c r="AS10" s="63"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="G11" s="83" t="s">
+      <c r="AQ10" s="90"/>
+      <c r="AR10" s="90"/>
+      <c r="AS10" s="91"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="G11" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="83">
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="57">
         <v>2</v>
       </c>
-      <c r="M11" s="84"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="77">
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="59">
         <f>R10+1</f>
         <v>43973</v>
       </c>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="77">
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="59">
         <f t="shared" si="0"/>
         <v>43976</v>
       </c>
-      <c r="S11" s="78"/>
-      <c r="T11" s="79"/>
-      <c r="U11" s="74" t="s">
+      <c r="S11" s="60"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="V11" s="75"/>
-      <c r="W11" s="76"/>
-      <c r="AR11" s="67"/>
-      <c r="AS11" s="67"/>
-      <c r="AT11" s="67"/>
-    </row>
-    <row r="12" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-    </row>
-    <row r="13" spans="1:55" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="Z13" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
-      <c r="AE13" s="41"/>
-      <c r="AF13" s="41"/>
-      <c r="AG13" s="41"/>
-      <c r="AH13" s="41"/>
-      <c r="AI13" s="46">
+      <c r="V11" s="72"/>
+      <c r="W11" s="73"/>
+      <c r="AR11" s="92"/>
+      <c r="AS11" s="92"/>
+      <c r="AT11" s="92"/>
+    </row>
+    <row r="12" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="1:55" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="Z13" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA13" s="78"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="78"/>
+      <c r="AE13" s="78"/>
+      <c r="AF13" s="78"/>
+      <c r="AG13" s="78"/>
+      <c r="AH13" s="78"/>
+      <c r="AI13" s="83">
         <f>SUM(AL10,AP10,Materiales!J20,'Costes Indirectos'!D7)</f>
-        <v>349702.29000000004</v>
-      </c>
-      <c r="AJ13" s="41"/>
-      <c r="AK13" s="41"/>
-      <c r="AL13" s="41"/>
-      <c r="AM13" s="41"/>
-      <c r="AN13" s="41"/>
-      <c r="AO13" s="41"/>
-      <c r="AP13" s="41"/>
-      <c r="AQ13" s="41"/>
-      <c r="AR13" s="41"/>
-      <c r="AS13" s="41"/>
-      <c r="AT13" s="41"/>
-      <c r="AU13" s="41"/>
-      <c r="AV13" s="47"/>
-      <c r="AW13" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX13" s="51"/>
-      <c r="AY13" s="51"/>
-      <c r="AZ13" s="51"/>
-      <c r="BA13" s="51"/>
-      <c r="BB13" s="51"/>
-      <c r="BC13" s="51"/>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="Z14" s="42"/>
-      <c r="AA14" s="43"/>
-      <c r="AB14" s="43"/>
-      <c r="AC14" s="43"/>
-      <c r="AD14" s="43"/>
-      <c r="AE14" s="43"/>
-      <c r="AF14" s="43"/>
-      <c r="AG14" s="43"/>
-      <c r="AH14" s="43"/>
-      <c r="AI14" s="43"/>
-      <c r="AJ14" s="43"/>
-      <c r="AK14" s="43"/>
-      <c r="AL14" s="43"/>
-      <c r="AM14" s="43"/>
-      <c r="AN14" s="43"/>
-      <c r="AO14" s="43"/>
-      <c r="AP14" s="43"/>
-      <c r="AQ14" s="43"/>
-      <c r="AR14" s="43"/>
-      <c r="AS14" s="43"/>
-      <c r="AT14" s="43"/>
-      <c r="AU14" s="43"/>
-      <c r="AV14" s="48"/>
-      <c r="AW14" s="50"/>
-      <c r="AX14" s="51"/>
-      <c r="AY14" s="51"/>
-      <c r="AZ14" s="51"/>
-      <c r="BA14" s="51"/>
-      <c r="BB14" s="51"/>
-      <c r="BC14" s="51"/>
-    </row>
-    <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="Z15" s="44"/>
-      <c r="AA15" s="45"/>
-      <c r="AB15" s="45"/>
-      <c r="AC15" s="45"/>
-      <c r="AD15" s="45"/>
-      <c r="AE15" s="45"/>
-      <c r="AF15" s="45"/>
-      <c r="AG15" s="45"/>
-      <c r="AH15" s="45"/>
-      <c r="AI15" s="45"/>
-      <c r="AJ15" s="45"/>
-      <c r="AK15" s="45"/>
-      <c r="AL15" s="45"/>
-      <c r="AM15" s="45"/>
-      <c r="AN15" s="45"/>
-      <c r="AO15" s="45"/>
-      <c r="AP15" s="45"/>
-      <c r="AQ15" s="45"/>
-      <c r="AR15" s="45"/>
-      <c r="AS15" s="45"/>
-      <c r="AT15" s="45"/>
-      <c r="AU15" s="45"/>
-      <c r="AV15" s="49"/>
-      <c r="AW15" s="50"/>
-      <c r="AX15" s="51"/>
-      <c r="AY15" s="51"/>
-      <c r="AZ15" s="51"/>
-      <c r="BA15" s="51"/>
-      <c r="BB15" s="51"/>
-      <c r="BC15" s="51"/>
-    </row>
-    <row r="16" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:56" ht="34.5" x14ac:dyDescent="0.25">
+        <v>195150.28999999998</v>
+      </c>
+      <c r="AJ13" s="78"/>
+      <c r="AK13" s="78"/>
+      <c r="AL13" s="78"/>
+      <c r="AM13" s="78"/>
+      <c r="AN13" s="78"/>
+      <c r="AO13" s="78"/>
+      <c r="AP13" s="78"/>
+      <c r="AQ13" s="78"/>
+      <c r="AR13" s="78"/>
+      <c r="AS13" s="78"/>
+      <c r="AT13" s="78"/>
+      <c r="AU13" s="78"/>
+      <c r="AV13" s="84"/>
+      <c r="AW13" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX13" s="88"/>
+      <c r="AY13" s="88"/>
+      <c r="AZ13" s="88"/>
+      <c r="BA13" s="88"/>
+      <c r="BB13" s="88"/>
+      <c r="BC13" s="88"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="Z14" s="79"/>
+      <c r="AA14" s="80"/>
+      <c r="AB14" s="80"/>
+      <c r="AC14" s="80"/>
+      <c r="AD14" s="80"/>
+      <c r="AE14" s="80"/>
+      <c r="AF14" s="80"/>
+      <c r="AG14" s="80"/>
+      <c r="AH14" s="80"/>
+      <c r="AI14" s="80"/>
+      <c r="AJ14" s="80"/>
+      <c r="AK14" s="80"/>
+      <c r="AL14" s="80"/>
+      <c r="AM14" s="80"/>
+      <c r="AN14" s="80"/>
+      <c r="AO14" s="80"/>
+      <c r="AP14" s="80"/>
+      <c r="AQ14" s="80"/>
+      <c r="AR14" s="80"/>
+      <c r="AS14" s="80"/>
+      <c r="AT14" s="80"/>
+      <c r="AU14" s="80"/>
+      <c r="AV14" s="85"/>
+      <c r="AW14" s="87"/>
+      <c r="AX14" s="88"/>
+      <c r="AY14" s="88"/>
+      <c r="AZ14" s="88"/>
+      <c r="BA14" s="88"/>
+      <c r="BB14" s="88"/>
+      <c r="BC14" s="88"/>
+    </row>
+    <row r="15" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="82"/>
+      <c r="AB15" s="82"/>
+      <c r="AC15" s="82"/>
+      <c r="AD15" s="82"/>
+      <c r="AE15" s="82"/>
+      <c r="AF15" s="82"/>
+      <c r="AG15" s="82"/>
+      <c r="AH15" s="82"/>
+      <c r="AI15" s="82"/>
+      <c r="AJ15" s="82"/>
+      <c r="AK15" s="82"/>
+      <c r="AL15" s="82"/>
+      <c r="AM15" s="82"/>
+      <c r="AN15" s="82"/>
+      <c r="AO15" s="82"/>
+      <c r="AP15" s="82"/>
+      <c r="AQ15" s="82"/>
+      <c r="AR15" s="82"/>
+      <c r="AS15" s="82"/>
+      <c r="AT15" s="82"/>
+      <c r="AU15" s="82"/>
+      <c r="AV15" s="86"/>
+      <c r="AW15" s="87"/>
+      <c r="AX15" s="88"/>
+      <c r="AY15" s="88"/>
+      <c r="AZ15" s="88"/>
+      <c r="BA15" s="88"/>
+      <c r="BB15" s="88"/>
+      <c r="BC15" s="88"/>
+    </row>
+    <row r="16" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:56" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="37">
         <v>43922</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>43976</v>
       </c>
     </row>
-    <row r="18" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -2567,7 +2568,7 @@
       <c r="BC18" s="38"/>
       <c r="BD18" s="38"/>
     </row>
-    <row r="19" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
@@ -2624,7 +2625,7 @@
       <c r="BC19" s="38"/>
       <c r="BD19" s="38"/>
     </row>
-    <row r="20" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
@@ -2681,7 +2682,7 @@
       <c r="BC20" s="38"/>
       <c r="BD20" s="38"/>
     </row>
-    <row r="21" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -2738,7 +2739,7 @@
       <c r="BC21" s="38"/>
       <c r="BD21" s="38"/>
     </row>
-    <row r="22" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -2795,7 +2796,7 @@
       <c r="BC22" s="38"/>
       <c r="BD22" s="38"/>
     </row>
-    <row r="23" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -2852,333 +2853,369 @@
       <c r="BC23" s="38"/>
       <c r="BD23" s="38"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="36"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="36"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C61" s="36"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="36"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="36"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="36"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="36"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="36"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="36"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="36"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C77" s="36"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C79" s="36"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C81" s="36"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="36"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C83" s="36"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="36"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C85" s="36"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="36"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C87" s="36"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="36"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C89" s="36"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="36"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="36"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="36"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C95" s="36"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C97" s="36"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C99" s="36"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C101" s="36"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="36"/>
       <c r="C103" s="36"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="36"/>
       <c r="C105" s="36"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C107" s="36"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="36"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="36"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C116" s="36"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="36"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C118" s="36"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="36"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="36"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="36"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C124" s="36"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="36"/>
       <c r="C126" s="36"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="36"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C130" s="36"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="36"/>
       <c r="C132" s="36"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="36"/>
       <c r="C134" s="36"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="36"/>
       <c r="C136" s="36"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="36"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C139" s="36"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="36"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C141" s="36"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C145" s="36"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C147" s="36"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="36"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C149" s="36"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C151" s="36"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C153" s="36"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="36"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="36"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C161" s="36"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="36"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C168" s="36"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C170" s="36"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="36"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="36"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C179" s="36"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="36"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="36"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="36"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C188" s="36"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="36"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C190" s="36"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="36"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="36"/>
       <c r="C194" s="36"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C197" s="36"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C200" s="36"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="36"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C202" s="36"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="36"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C204" s="36"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="36"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="36"/>
       <c r="C207" s="36"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="36"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="36"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="36"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C214" s="36"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="36"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C216" s="36"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="36"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C218" s="36"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C220" s="36"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="36"/>
       <c r="C222" s="36"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C224" s="36"/>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C226" s="36"/>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C228" s="36"/>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C230" s="36"/>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C235" s="36"/>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="36"/>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="36"/>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="36"/>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C252" s="36"/>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C254" s="36"/>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C256" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="Z13:AH15"/>
+    <mergeCell ref="AI13:AV15"/>
+    <mergeCell ref="AW13:BC15"/>
+    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AP6:AS6"/>
+    <mergeCell ref="AP7:AS7"/>
+    <mergeCell ref="AP8:AS8"/>
+    <mergeCell ref="AP9:AS9"/>
+    <mergeCell ref="AP10:AS10"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AR11:AT11"/>
+    <mergeCell ref="AL6:AO6"/>
+    <mergeCell ref="AL10:AO10"/>
+    <mergeCell ref="AI10:AK10"/>
+    <mergeCell ref="AL5:AO5"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="AI6:AK6"/>
+    <mergeCell ref="AI7:AK7"/>
+    <mergeCell ref="AI8:AK8"/>
+    <mergeCell ref="AI9:AK9"/>
+    <mergeCell ref="AC7:AH7"/>
+    <mergeCell ref="AC6:AH6"/>
+    <mergeCell ref="AC8:AH8"/>
+    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AI5:AK5"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="R5:T5"/>
@@ -3195,52 +3232,16 @@
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="AI6:AK6"/>
-    <mergeCell ref="AI7:AK7"/>
-    <mergeCell ref="AI8:AK8"/>
-    <mergeCell ref="AI9:AK9"/>
-    <mergeCell ref="AC7:AH7"/>
-    <mergeCell ref="AC6:AH6"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="AC9:AH9"/>
-    <mergeCell ref="AI5:AK5"/>
-    <mergeCell ref="Z13:AH15"/>
-    <mergeCell ref="AI13:AV15"/>
-    <mergeCell ref="AW13:BC15"/>
-    <mergeCell ref="AP5:AS5"/>
-    <mergeCell ref="AP6:AS6"/>
-    <mergeCell ref="AP7:AS7"/>
-    <mergeCell ref="AP8:AS8"/>
-    <mergeCell ref="AP9:AS9"/>
-    <mergeCell ref="AP10:AS10"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AR11:AT11"/>
-    <mergeCell ref="AL6:AO6"/>
-    <mergeCell ref="AL10:AO10"/>
-    <mergeCell ref="AI10:AK10"/>
-    <mergeCell ref="AL5:AO5"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:BD23">
     <cfRule type="expression" dxfId="1" priority="15">
@@ -3259,74 +3260,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B6B2AB-6A6F-45AD-8EE8-E01836CACEB7}">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="40.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
     <col min="17" max="17" width="32" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="107" t="s">
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="108"/>
-    </row>
-    <row r="4" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="109"/>
-      <c r="C4" s="110"/>
-      <c r="E4" s="107" t="s">
+      <c r="C3" s="96"/>
+    </row>
+    <row r="4" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="97"/>
+      <c r="C4" s="98"/>
+      <c r="E4" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="108"/>
+      <c r="F4" s="96"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="111" t="s">
+      <c r="H4" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="K4" s="99" t="s">
+      <c r="I4" s="100"/>
+      <c r="K4" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="100"/>
-      <c r="N4" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="O4" s="100"/>
-      <c r="Q4" s="99" t="s">
+      <c r="L4" s="116"/>
+      <c r="N4" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="116"/>
+      <c r="Q4" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="100"/>
-    </row>
-    <row r="5" spans="2:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="117"/>
-      <c r="C5" s="118"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="110"/>
+      <c r="R4" s="116"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="105"/>
+      <c r="C5" s="106"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="114"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="N5" s="101"/>
-      <c r="O5" s="102"/>
-      <c r="Q5" s="101"/>
-      <c r="R5" s="102"/>
-    </row>
-    <row r="6" spans="2:18" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="118"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="118"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="118"/>
+    </row>
+    <row r="6" spans="2:18" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>149.99</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>19.97</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="17" t="s">
         <v>31</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>500 €/mes</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="26"/>
       <c r="C9" s="27"/>
       <c r="E9" s="3" t="s">
@@ -3483,11 +3484,11 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="115" t="s">
+    <row r="10" spans="2:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="116"/>
+      <c r="C10" s="104"/>
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
@@ -3522,7 +3523,7 @@
         <v>6005</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
         <v>33</v>
       </c>
@@ -3563,7 +3564,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
@@ -3600,15 +3601,15 @@
         <v>8029.96</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="117"/>
-      <c r="C13" s="118"/>
+    <row r="13" spans="2:18" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="105"/>
+      <c r="C13" s="106"/>
       <c r="E13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="22">
         <f>C35*3</f>
-        <v>162149.13</v>
+        <v>21149.13</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>7</v>
@@ -3627,11 +3628,11 @@
         <v>4172.13</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="115" t="s">
+    <row r="14" spans="2:18" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="116"/>
+      <c r="C14" s="104"/>
       <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
@@ -3650,7 +3651,7 @@
       <c r="Q14" s="39"/>
       <c r="R14" s="39"/>
     </row>
-    <row r="15" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
         <v>35</v>
       </c>
@@ -3664,14 +3665,14 @@
         <f>C36*70+C37*25</f>
         <v>981.80000000000007</v>
       </c>
-      <c r="H15" s="103" t="s">
+      <c r="H15" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="104"/>
+      <c r="I15" s="120"/>
       <c r="K15" s="10"/>
       <c r="L15" s="7"/>
       <c r="N15" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O15" s="22">
         <f>2*309.99</f>
@@ -3680,7 +3681,7 @@
       <c r="Q15" s="39"/>
       <c r="R15" s="39"/>
     </row>
-    <row r="16" spans="2:18" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
         <v>42</v>
       </c>
@@ -3692,10 +3693,10 @@
       </c>
       <c r="F16" s="29">
         <f>SUM(F6:F15)</f>
-        <v>192566.88</v>
-      </c>
-      <c r="H16" s="105"/>
-      <c r="I16" s="106"/>
+        <v>51566.880000000005</v>
+      </c>
+      <c r="H16" s="121"/>
+      <c r="I16" s="122"/>
       <c r="N16" s="8" t="s">
         <v>7</v>
       </c>
@@ -3704,7 +3705,7 @@
         <v>69728.659999999989</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>45</v>
       </c>
@@ -3720,7 +3721,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>36</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>38</v>
       </c>
@@ -3739,46 +3740,46 @@
         <v>1608.3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="22">
         <v>1114.08</v>
       </c>
-      <c r="H20" s="119" t="s">
+      <c r="H20" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="120"/>
-      <c r="J20" s="95">
+      <c r="I20" s="108"/>
+      <c r="J20" s="111">
         <f>SUM(F16,I13,I17,L11,O16,R12)</f>
-        <v>274531.29000000004</v>
-      </c>
-      <c r="K20" s="96"/>
-    </row>
-    <row r="21" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133531.28999999998</v>
+      </c>
+      <c r="K20" s="112"/>
+    </row>
+    <row r="21" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="18">
         <v>509</v>
       </c>
-      <c r="H21" s="121"/>
-      <c r="I21" s="122"/>
-      <c r="J21" s="97"/>
-      <c r="K21" s="98"/>
-    </row>
-    <row r="22" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="117"/>
-      <c r="C22" s="118"/>
-    </row>
-    <row r="23" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H21" s="109"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="114"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="105"/>
+      <c r="C22" s="106"/>
+    </row>
+    <row r="23" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="14"/>
     </row>
-    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
         <v>40</v>
       </c>
@@ -3786,7 +3787,7 @@
         <v>59.02</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="19" t="s">
         <v>41</v>
       </c>
@@ -3794,21 +3795,21 @@
         <v>43.64</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
-    </row>
-    <row r="27" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="107" t="s">
+    <row r="26" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="105"/>
+      <c r="C26" s="106"/>
+    </row>
+    <row r="27" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="108"/>
-    </row>
-    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="109"/>
-      <c r="C28" s="110"/>
-    </row>
-    <row r="29" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="96"/>
+    </row>
+    <row r="28" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="97"/>
+      <c r="C28" s="98"/>
+    </row>
+    <row r="29" spans="2:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>58</v>
       </c>
@@ -3816,7 +3817,7 @@
         <v>19.97</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>59</v>
       </c>
@@ -3824,7 +3825,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>60</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>1199.99</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>63</v>
       </c>
@@ -3856,15 +3857,15 @@
         <v>4674</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C35" s="22">
-        <v>54049.71</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7049.71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
         <v>65</v>
       </c>
@@ -3872,7 +3873,7 @@
         <v>10.99</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="28" t="s">
         <v>66</v>
       </c>
@@ -3880,9 +3881,14 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J20:K21"/>
+    <mergeCell ref="K4:L5"/>
+    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="Q4:R5"/>
+    <mergeCell ref="H15:I16"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="H4:I5"/>
     <mergeCell ref="B27:C28"/>
@@ -3894,11 +3900,6 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="H20:I21"/>
     <mergeCell ref="E4:F5"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="K4:L5"/>
-    <mergeCell ref="N4:O5"/>
-    <mergeCell ref="Q4:R5"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://www.dell.com/es-es/work/shop/accessories/apd/210-APWV" xr:uid="{A7CA1EDC-A29D-41BB-84C7-1EC45A4421FB}"/>
@@ -3937,7 +3938,7 @@
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3958,29 +3959,29 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="123" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" s="123"/>
       <c r="D3" s="123"/>
       <c r="E3" s="123"/>
     </row>
-    <row r="6" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-    </row>
-    <row r="7" spans="3:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+    </row>
+    <row r="7" spans="3:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="12" t="s">
         <v>72</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F6:G6"/>
@@ -4014,56 +4015,56 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="123" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="123"/>
       <c r="D3" s="123"/>
       <c r="E3" s="123"/>
     </row>
-    <row r="5" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="3:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="115" t="s">
+    <row r="5" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="3:5" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="116"/>
-    </row>
-    <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="104"/>
+    </row>
+    <row r="7" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="16">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D9" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="11" t="s">
         <v>68</v>
       </c>
@@ -4088,25 +4089,25 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="123" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="123"/>
       <c r="D3" s="123"/>
       <c r="E3" s="123"/>
     </row>
-    <row r="6" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="3:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="3:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>87</v>
       </c>
@@ -4114,7 +4115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="12" t="s">
         <v>88</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:E3"/>

</xml_diff>

<commit_message>
Reformas parte 3: Docimentdo esquema de red, reducido presupuesto, mauqetando Edificio
</commit_message>
<xml_diff>
--- a/fol/UBALDE_Presupuesto.xlsx
+++ b/fol/UBALDE_Presupuesto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerjox\Repos\2h\fol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\repos\2h\fol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C68EE-A7A6-418A-A01C-B6A42177C974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B5F01-64DB-464B-A114-3090ADEFDDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="20865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Construcción edificio" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="103">
   <si>
     <t>CPD</t>
   </si>
@@ -62,12 +62,6 @@
     <t>x2 Routers</t>
   </si>
   <si>
-    <t>x4 Switches</t>
-  </si>
-  <si>
-    <t>x2 NAS</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>Patch panels</t>
   </si>
   <si>
-    <t>x3 Servidores</t>
-  </si>
-  <si>
     <t>x70 Latiguillos + 25 Fibra</t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>SOFTWARE</t>
   </si>
   <si>
-    <t>Windows Server 2019 Datacenter</t>
-  </si>
-  <si>
     <t>Windows Server 2019 Standard</t>
   </si>
   <si>
@@ -308,9 +296,6 @@
     <t>Equipos informáticos</t>
   </si>
   <si>
-    <t>x2 Impresoras</t>
-  </si>
-  <si>
     <t>Router (Unifi Dream Machine Pro)</t>
   </si>
   <si>
@@ -360,6 +345,18 @@
   </si>
   <si>
     <t>Sistemas</t>
+  </si>
+  <si>
+    <t>x1 NAS</t>
+  </si>
+  <si>
+    <t>x5 Switches</t>
+  </si>
+  <si>
+    <t>Impresoras</t>
+  </si>
+  <si>
+    <t>x2 Servidores</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1244,278 +1241,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1525,28 +1277,275 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1600,7 +1599,7 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1929,566 +1928,566 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD261A9-C307-498A-9ABC-0594443A472D}">
   <dimension ref="A1:BD256"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="38" width="3.42578125" customWidth="1"/>
-    <col min="39" max="43" width="3.5703125" customWidth="1"/>
-    <col min="44" max="44" width="3.7109375" customWidth="1"/>
-    <col min="45" max="45" width="3.28515625" customWidth="1"/>
-    <col min="46" max="47" width="3.5703125" customWidth="1"/>
-    <col min="48" max="48" width="3.42578125" customWidth="1"/>
-    <col min="49" max="49" width="3.28515625" customWidth="1"/>
-    <col min="50" max="55" width="3.42578125" customWidth="1"/>
-    <col min="56" max="56" width="3.140625" customWidth="1"/>
-    <col min="57" max="60" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="5" width="3.88671875" customWidth="1"/>
+    <col min="6" max="38" width="3.44140625" customWidth="1"/>
+    <col min="39" max="43" width="3.5546875" customWidth="1"/>
+    <col min="44" max="44" width="3.6640625" customWidth="1"/>
+    <col min="45" max="45" width="3.33203125" customWidth="1"/>
+    <col min="46" max="47" width="3.5546875" customWidth="1"/>
+    <col min="48" max="48" width="3.44140625" customWidth="1"/>
+    <col min="49" max="49" width="3.33203125" customWidth="1"/>
+    <col min="50" max="55" width="3.44140625" customWidth="1"/>
+    <col min="56" max="56" width="3.109375" customWidth="1"/>
+    <col min="57" max="60" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
     </row>
-    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:55" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AC3" s="130" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD3" s="131"/>
-      <c r="AE3" s="131"/>
-      <c r="AF3" s="131"/>
-      <c r="AG3" s="131"/>
-      <c r="AH3" s="131"/>
-      <c r="AI3" s="131"/>
-      <c r="AJ3" s="131"/>
-      <c r="AK3" s="131"/>
-      <c r="AL3" s="131"/>
-      <c r="AM3" s="131"/>
-      <c r="AN3" s="131"/>
-      <c r="AO3" s="132"/>
-      <c r="AP3" s="129"/>
-      <c r="AQ3" s="129"/>
-      <c r="AR3" s="129"/>
-      <c r="AS3" s="129"/>
-    </row>
-    <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AC4" s="129"/>
-      <c r="AD4" s="129"/>
-      <c r="AE4" s="129"/>
-      <c r="AF4" s="129"/>
-      <c r="AG4" s="129"/>
-      <c r="AH4" s="129"/>
-      <c r="AI4" s="129"/>
-      <c r="AJ4" s="129"/>
-      <c r="AK4" s="129"/>
-      <c r="AL4" s="129"/>
-      <c r="AM4" s="129"/>
-      <c r="AN4" s="129"/>
-      <c r="AO4" s="129"/>
-      <c r="AP4" s="129"/>
-      <c r="AQ4" s="129"/>
-      <c r="AR4" s="129"/>
-      <c r="AS4" s="129"/>
-    </row>
-    <row r="5" spans="1:55" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="82" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="G5" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="79" t="s">
+    <row r="2" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:55" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC3" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="52"/>
+      <c r="AI3" s="52"/>
+      <c r="AJ3" s="52"/>
+      <c r="AK3" s="52"/>
+      <c r="AL3" s="52"/>
+      <c r="AM3" s="52"/>
+      <c r="AN3" s="52"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="41"/>
+      <c r="AQ3" s="41"/>
+      <c r="AR3" s="41"/>
+      <c r="AS3" s="41"/>
+    </row>
+    <row r="4" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="41"/>
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="41"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="41"/>
+      <c r="AR4" s="41"/>
+      <c r="AS4" s="41"/>
+    </row>
+    <row r="5" spans="1:55" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="G5" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
-      <c r="O5" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="48" t="s">
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" s="63"/>
+      <c r="T5" s="64"/>
+      <c r="U5" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="V5" s="89"/>
+      <c r="W5" s="90"/>
+      <c r="AI5" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ5" s="92"/>
+      <c r="AK5" s="93"/>
+      <c r="AL5" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM5" s="107"/>
+      <c r="AN5" s="107"/>
+      <c r="AO5" s="108"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B6" s="56">
+        <v>43930</v>
+      </c>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="G6" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="V5" s="64"/>
-      <c r="W5" s="65"/>
-      <c r="AI5" s="116" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ5" s="117"/>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="119" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM5" s="120"/>
-      <c r="AN5" s="120"/>
-      <c r="AO5" s="121"/>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="83">
-        <v>43930</v>
-      </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="G6" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="77">
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="68">
         <v>2</v>
       </c>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="72">
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="65">
         <v>43922</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="72">
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="65">
         <f t="shared" ref="R6:R11" si="0">WORKDAY(O6-1,L6,$B$6:$E$15)</f>
         <v>43923</v>
       </c>
-      <c r="S6" s="73"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="51" t="s">
+      <c r="S6" s="66"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="V6" s="80"/>
+      <c r="W6" s="81"/>
+      <c r="AC6" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="V6" s="52"/>
-      <c r="W6" s="53"/>
-      <c r="AC6" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD6" s="52"/>
-      <c r="AE6" s="52"/>
-      <c r="AF6" s="52"/>
-      <c r="AG6" s="52"/>
-      <c r="AH6" s="53"/>
-      <c r="AI6" s="51">
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="80"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="81"/>
+      <c r="AI6" s="79">
         <v>3</v>
       </c>
-      <c r="AJ6" s="52"/>
-      <c r="AK6" s="53"/>
-      <c r="AL6" s="57">
+      <c r="AJ6" s="80"/>
+      <c r="AK6" s="81"/>
+      <c r="AL6" s="75">
         <f>SUM(IF(COUNTIF($U$6,"*R*"),(AI6*'Otros Costes'!G5)*$L$6,0),IF(COUNTIF($U$7,"*R*"),(AI6*'Otros Costes'!G5)*$L$7,0),IF(COUNTIF($U$8,"*R*"),(AI6*'Otros Costes'!G5)*$L$8,0),IF(COUNTIF($U$9,"*R*"),(AI6*'Otros Costes'!G5)*$L$9,0),IF(COUNTIF($U$10,"*R*"),(AI6*'Otros Costes'!G5)*$L$10,0),IF(COUNTIF($U$11,"*R*"),(AI6*'Otros Costes'!G5)*$L$11,0))</f>
         <v>2652</v>
       </c>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="59"/>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B7" s="83">
+      <c r="AM6" s="76"/>
+      <c r="AN6" s="76"/>
+      <c r="AO6" s="77"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B7" s="56">
         <v>43931</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="G7" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="77">
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="G7" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="68">
         <v>14</v>
       </c>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="72">
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="65">
         <f>R6+1</f>
         <v>43924</v>
       </c>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="72">
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="65">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="S7" s="73"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="V7" s="55"/>
-      <c r="W7" s="56"/>
-      <c r="AC7" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD7" s="55"/>
-      <c r="AE7" s="55"/>
-      <c r="AF7" s="55"/>
-      <c r="AG7" s="55"/>
-      <c r="AH7" s="56"/>
-      <c r="AI7" s="54">
+      <c r="S7" s="66"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="V7" s="83"/>
+      <c r="W7" s="84"/>
+      <c r="AC7" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="84"/>
+      <c r="AI7" s="82">
         <v>3</v>
       </c>
-      <c r="AJ7" s="55"/>
-      <c r="AK7" s="56"/>
-      <c r="AL7" s="57">
+      <c r="AJ7" s="83"/>
+      <c r="AK7" s="84"/>
+      <c r="AL7" s="75">
         <f>SUM(IF(COUNTIF($U$6,"*E*"),(AI7*'Otros Costes'!G6)*$L$6,0),IF(COUNTIF($U$7,"*E*"),(AI7*'Otros Costes'!G6)*$L$7,0),IF(COUNTIF($U$8,"*E*"),(AI7*'Otros Costes'!G6)*$L$8,0),IF(COUNTIF($U$9,"*E*"),(AI7*'Otros Costes'!G6)*$L$9,0),IF(COUNTIF($U$10,"*E*"),(AI7*'Otros Costes'!G6)*$L$10,0),IF(COUNTIF($U$11,"*E*"),(AI7*'Otros Costes'!G6)*$L$11,0))</f>
         <v>2016</v>
       </c>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="59"/>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B8" s="83">
+      <c r="AM7" s="76"/>
+      <c r="AN7" s="76"/>
+      <c r="AO7" s="77"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B8" s="56">
         <v>43934</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="G8" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="77">
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="G8" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="68">
         <v>7</v>
       </c>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="72">
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="65">
         <f>R7+1</f>
         <v>43949</v>
       </c>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="72">
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="65">
         <f t="shared" si="0"/>
         <v>43957</v>
       </c>
-      <c r="S8" s="73"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="V8" s="55"/>
-      <c r="W8" s="56"/>
-      <c r="AC8" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD8" s="55"/>
-      <c r="AE8" s="55"/>
-      <c r="AF8" s="55"/>
-      <c r="AG8" s="55"/>
-      <c r="AH8" s="56"/>
-      <c r="AI8" s="54">
+      <c r="S8" s="66"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="V8" s="83"/>
+      <c r="W8" s="84"/>
+      <c r="AC8" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="84"/>
+      <c r="AI8" s="82">
         <v>3</v>
       </c>
-      <c r="AJ8" s="55"/>
-      <c r="AK8" s="56"/>
-      <c r="AL8" s="57">
+      <c r="AJ8" s="83"/>
+      <c r="AK8" s="84"/>
+      <c r="AL8" s="75">
         <f>SUM(IF(COUNTIF($U$6,"*T*"),(AI8*'Otros Costes'!G7)*$L$6,0),IF(COUNTIF($U$7,"*T*"),(AI8*'Otros Costes'!G7)*$L$7,0),IF(COUNTIF($U$8,"*T*"),(AI8*'Otros Costes'!G7)*$L$8,0),IF(COUNTIF($U$9,"*T*"),(AI8*'Otros Costes'!G7)*$L$9,0),IF(COUNTIF($U$10,"*T*"),(AI8*'Otros Costes'!G7)*$L$10,0),IF(COUNTIF($U$11,"*T*"),(AI8*'Otros Costes'!G7)*$L$11,0))</f>
         <v>672</v>
       </c>
-      <c r="AM8" s="58"/>
-      <c r="AN8" s="58"/>
-      <c r="AO8" s="59"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B9" s="84">
+      <c r="AM8" s="76"/>
+      <c r="AN8" s="76"/>
+      <c r="AO8" s="77"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B9" s="57">
         <v>43974</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="86"/>
-      <c r="G9" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="77">
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="G9" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="68">
         <v>7</v>
       </c>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="72">
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="65">
         <f>R8+1</f>
         <v>43958</v>
       </c>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="72">
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="65">
         <f t="shared" si="0"/>
         <v>43966</v>
       </c>
-      <c r="S9" s="73"/>
-      <c r="T9" s="74"/>
-      <c r="U9" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="AC9" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD9" s="67"/>
-      <c r="AE9" s="67"/>
-      <c r="AF9" s="67"/>
-      <c r="AG9" s="67"/>
-      <c r="AH9" s="67"/>
-      <c r="AI9" s="66">
+      <c r="S9" s="66"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" s="83"/>
+      <c r="W9" s="84"/>
+      <c r="AC9" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="86"/>
+      <c r="AE9" s="86"/>
+      <c r="AF9" s="86"/>
+      <c r="AG9" s="86"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="85">
         <v>1</v>
       </c>
-      <c r="AJ9" s="67"/>
-      <c r="AK9" s="68"/>
-      <c r="AL9" s="58">
+      <c r="AJ9" s="86"/>
+      <c r="AK9" s="87"/>
+      <c r="AL9" s="76">
         <f>SUM(IF(COUNTIF($U$6,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$6,0),IF(COUNTIF($U$7,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$7,0),IF(COUNTIF($U$8,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$8,0),IF(COUNTIF($U$9,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$9,0),IF(COUNTIF($U$10,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$10,0),IF(COUNTIF($U$11,"*CAP*"),(AI9*'Otros Costes'!G8)*$L$11,0))</f>
         <v>736</v>
       </c>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="58"/>
-      <c r="AO9" s="59"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="86"/>
-      <c r="G10" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="77">
+      <c r="AM9" s="76"/>
+      <c r="AN9" s="76"/>
+      <c r="AO9" s="77"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B10" s="57"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="G10" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="68">
         <v>4</v>
       </c>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="72">
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="65">
         <f>R9+1</f>
         <v>43967</v>
       </c>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="72">
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="65">
         <f t="shared" si="0"/>
         <v>43972</v>
       </c>
-      <c r="S10" s="73"/>
-      <c r="T10" s="74"/>
-      <c r="U10" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="V10" s="55"/>
-      <c r="W10" s="56"/>
-      <c r="AI10" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ10" s="62"/>
-      <c r="AK10" s="62"/>
-      <c r="AL10" s="60">
+      <c r="S10" s="66"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="V10" s="83"/>
+      <c r="W10" s="84"/>
+      <c r="AI10" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="105"/>
+      <c r="AK10" s="105"/>
+      <c r="AL10" s="104">
         <f>SUM(AL6:AO9)</f>
         <v>6076</v>
       </c>
-      <c r="AM10" s="61"/>
-      <c r="AN10" s="61"/>
-      <c r="AO10" s="61"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="G11" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="75">
+      <c r="AM10" s="54"/>
+      <c r="AN10" s="54"/>
+      <c r="AO10" s="54"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="G11" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="71">
         <v>2</v>
       </c>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="69">
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="73">
         <f>R10+1</f>
         <v>43973</v>
       </c>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="69">
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="73">
         <f t="shared" si="0"/>
         <v>43976</v>
       </c>
-      <c r="S11" s="70"/>
-      <c r="T11" s="71"/>
-      <c r="U11" s="66" t="s">
-        <v>77</v>
-      </c>
-      <c r="V11" s="67"/>
-      <c r="W11" s="68"/>
-      <c r="AT11" s="125"/>
-    </row>
-    <row r="12" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="G12" s="122" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="123"/>
-      <c r="O12" s="123"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="123"/>
-      <c r="S12" s="123"/>
-      <c r="T12" s="123"/>
-      <c r="U12" s="123"/>
-      <c r="V12" s="123"/>
-      <c r="W12" s="124"/>
-    </row>
-    <row r="13" spans="1:55" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="Z13" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA13" s="39"/>
-      <c r="AB13" s="39"/>
-      <c r="AC13" s="39"/>
-      <c r="AD13" s="39"/>
-      <c r="AE13" s="39"/>
-      <c r="AF13" s="39"/>
-      <c r="AG13" s="39"/>
-      <c r="AH13" s="39"/>
-      <c r="AI13" s="44">
+      <c r="S11" s="74"/>
+      <c r="T11" s="78"/>
+      <c r="U11" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="V11" s="86"/>
+      <c r="W11" s="87"/>
+      <c r="AT11" s="39"/>
+    </row>
+    <row r="12" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="G12" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="50"/>
+    </row>
+    <row r="13" spans="1:55" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="Z13" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA13" s="95"/>
+      <c r="AB13" s="95"/>
+      <c r="AC13" s="95"/>
+      <c r="AD13" s="95"/>
+      <c r="AE13" s="95"/>
+      <c r="AF13" s="95"/>
+      <c r="AG13" s="95"/>
+      <c r="AH13" s="95"/>
+      <c r="AI13" s="100">
         <f>SUM(AL10,Materiales!J20)</f>
-        <v>68116.069999999992</v>
-      </c>
-      <c r="AJ13" s="39"/>
-      <c r="AK13" s="39"/>
-      <c r="AL13" s="39"/>
-      <c r="AM13" s="39"/>
-      <c r="AN13" s="39"/>
-      <c r="AO13" s="39"/>
-      <c r="AP13" s="39"/>
-      <c r="AQ13" s="39"/>
-      <c r="AR13" s="39"/>
-      <c r="AS13" s="39"/>
-      <c r="AT13" s="39"/>
-      <c r="AU13" s="39"/>
-      <c r="AV13" s="45"/>
-      <c r="AW13" s="133"/>
-      <c r="AX13" s="134"/>
-      <c r="AY13" s="134"/>
-      <c r="AZ13" s="134"/>
-      <c r="BA13" s="134"/>
-      <c r="BB13" s="134"/>
-      <c r="BC13" s="134"/>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="41"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="41"/>
-      <c r="AG14" s="41"/>
-      <c r="AH14" s="41"/>
-      <c r="AI14" s="41"/>
-      <c r="AJ14" s="41"/>
-      <c r="AK14" s="41"/>
-      <c r="AL14" s="41"/>
-      <c r="AM14" s="41"/>
-      <c r="AN14" s="41"/>
-      <c r="AO14" s="41"/>
-      <c r="AP14" s="41"/>
-      <c r="AQ14" s="41"/>
-      <c r="AR14" s="41"/>
-      <c r="AS14" s="41"/>
-      <c r="AT14" s="41"/>
-      <c r="AU14" s="41"/>
-      <c r="AV14" s="46"/>
-      <c r="AW14" s="133"/>
-      <c r="AX14" s="134"/>
-      <c r="AY14" s="134"/>
-      <c r="AZ14" s="134"/>
-      <c r="BA14" s="134"/>
-      <c r="BB14" s="134"/>
-      <c r="BC14" s="134"/>
-    </row>
-    <row r="15" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="Z15" s="42"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="43"/>
-      <c r="AC15" s="43"/>
-      <c r="AD15" s="43"/>
-      <c r="AE15" s="43"/>
-      <c r="AF15" s="43"/>
-      <c r="AG15" s="43"/>
-      <c r="AH15" s="43"/>
-      <c r="AI15" s="43"/>
-      <c r="AJ15" s="43"/>
-      <c r="AK15" s="43"/>
-      <c r="AL15" s="43"/>
-      <c r="AM15" s="43"/>
-      <c r="AN15" s="43"/>
-      <c r="AO15" s="43"/>
-      <c r="AP15" s="43"/>
-      <c r="AQ15" s="43"/>
-      <c r="AR15" s="43"/>
-      <c r="AS15" s="43"/>
-      <c r="AT15" s="43"/>
-      <c r="AU15" s="43"/>
-      <c r="AV15" s="47"/>
-      <c r="AW15" s="133"/>
-      <c r="AX15" s="134"/>
-      <c r="AY15" s="134"/>
-      <c r="AZ15" s="134"/>
-      <c r="BA15" s="134"/>
-      <c r="BB15" s="134"/>
-      <c r="BC15" s="134"/>
-    </row>
-    <row r="16" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:56" ht="34.5" x14ac:dyDescent="0.25">
+        <v>55078.529999999992</v>
+      </c>
+      <c r="AJ13" s="95"/>
+      <c r="AK13" s="95"/>
+      <c r="AL13" s="95"/>
+      <c r="AM13" s="95"/>
+      <c r="AN13" s="95"/>
+      <c r="AO13" s="95"/>
+      <c r="AP13" s="95"/>
+      <c r="AQ13" s="95"/>
+      <c r="AR13" s="95"/>
+      <c r="AS13" s="95"/>
+      <c r="AT13" s="95"/>
+      <c r="AU13" s="95"/>
+      <c r="AV13" s="101"/>
+      <c r="AW13" s="42"/>
+      <c r="AX13" s="43"/>
+      <c r="AY13" s="43"/>
+      <c r="AZ13" s="43"/>
+      <c r="BA13" s="43"/>
+      <c r="BB13" s="43"/>
+      <c r="BC13" s="43"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="Z14" s="96"/>
+      <c r="AA14" s="97"/>
+      <c r="AB14" s="97"/>
+      <c r="AC14" s="97"/>
+      <c r="AD14" s="97"/>
+      <c r="AE14" s="97"/>
+      <c r="AF14" s="97"/>
+      <c r="AG14" s="97"/>
+      <c r="AH14" s="97"/>
+      <c r="AI14" s="97"/>
+      <c r="AJ14" s="97"/>
+      <c r="AK14" s="97"/>
+      <c r="AL14" s="97"/>
+      <c r="AM14" s="97"/>
+      <c r="AN14" s="97"/>
+      <c r="AO14" s="97"/>
+      <c r="AP14" s="97"/>
+      <c r="AQ14" s="97"/>
+      <c r="AR14" s="97"/>
+      <c r="AS14" s="97"/>
+      <c r="AT14" s="97"/>
+      <c r="AU14" s="97"/>
+      <c r="AV14" s="102"/>
+      <c r="AW14" s="42"/>
+      <c r="AX14" s="43"/>
+      <c r="AY14" s="43"/>
+      <c r="AZ14" s="43"/>
+      <c r="BA14" s="43"/>
+      <c r="BB14" s="43"/>
+      <c r="BC14" s="43"/>
+    </row>
+    <row r="15" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="99"/>
+      <c r="AB15" s="99"/>
+      <c r="AC15" s="99"/>
+      <c r="AD15" s="99"/>
+      <c r="AE15" s="99"/>
+      <c r="AF15" s="99"/>
+      <c r="AG15" s="99"/>
+      <c r="AH15" s="99"/>
+      <c r="AI15" s="99"/>
+      <c r="AJ15" s="99"/>
+      <c r="AK15" s="99"/>
+      <c r="AL15" s="99"/>
+      <c r="AM15" s="99"/>
+      <c r="AN15" s="99"/>
+      <c r="AO15" s="99"/>
+      <c r="AP15" s="99"/>
+      <c r="AQ15" s="99"/>
+      <c r="AR15" s="99"/>
+      <c r="AS15" s="99"/>
+      <c r="AT15" s="99"/>
+      <c r="AU15" s="99"/>
+      <c r="AV15" s="103"/>
+      <c r="AW15" s="42"/>
+      <c r="AX15" s="43"/>
+      <c r="AY15" s="43"/>
+      <c r="AZ15" s="43"/>
+      <c r="BA15" s="43"/>
+      <c r="BB15" s="43"/>
+      <c r="BC15" s="43"/>
+    </row>
+    <row r="16" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:56" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B17" s="35">
         <v>43922</v>
       </c>
@@ -2655,7 +2654,7 @@
         <v>43976</v>
       </c>
     </row>
-    <row r="18" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
@@ -2712,7 +2711,7 @@
       <c r="BC18" s="36"/>
       <c r="BD18" s="36"/>
     </row>
-    <row r="19" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
       <c r="D19" s="36"/>
@@ -2769,7 +2768,7 @@
       <c r="BC19" s="36"/>
       <c r="BD19" s="36"/>
     </row>
-    <row r="20" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
@@ -2826,7 +2825,7 @@
       <c r="BC20" s="36"/>
       <c r="BD20" s="36"/>
     </row>
-    <row r="21" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
@@ -2883,7 +2882,7 @@
       <c r="BC21" s="36"/>
       <c r="BD21" s="36"/>
     </row>
-    <row r="22" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
@@ -2940,7 +2939,7 @@
       <c r="BC22" s="36"/>
       <c r="BD22" s="36"/>
     </row>
-    <row r="23" spans="2:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:56" x14ac:dyDescent="0.3">
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
       <c r="D23" s="36"/>
@@ -2997,359 +2996,341 @@
       <c r="BC23" s="36"/>
       <c r="BD23" s="36"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="34"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="34"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C61" s="34"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="34"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="34"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="34"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="34"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="34"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="34"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="34"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C77" s="34"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C79" s="34"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C81" s="34"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="34"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C83" s="34"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="34"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C85" s="34"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="34"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C87" s="34"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="34"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C89" s="34"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="34"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="34"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="34"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C95" s="34"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C97" s="34"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C99" s="34"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C101" s="34"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="34"/>
       <c r="C103" s="34"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="34"/>
       <c r="C105" s="34"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C107" s="34"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="34"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="34"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C116" s="34"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="34"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C118" s="34"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="34"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="34"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="34"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C124" s="34"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="34"/>
       <c r="C126" s="34"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="34"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C130" s="34"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="34"/>
       <c r="C132" s="34"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="34"/>
       <c r="C134" s="34"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="34"/>
       <c r="C136" s="34"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="34"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C139" s="34"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="34"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C141" s="34"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C145" s="34"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C147" s="34"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="34"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C149" s="34"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C151" s="34"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C153" s="34"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="34"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="34"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C161" s="34"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="34"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C168" s="34"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C170" s="34"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="34"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="34"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C179" s="34"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="34"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="34"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="34"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C188" s="34"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="34"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C190" s="34"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="34"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="34"/>
       <c r="C194" s="34"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C197" s="34"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C200" s="34"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="34"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C202" s="34"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="34"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C204" s="34"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="34"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="34"/>
       <c r="C207" s="34"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="34"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="34"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="34"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C214" s="34"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="34"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C216" s="34"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="34"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C218" s="34"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C220" s="34"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="34"/>
       <c r="C222" s="34"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C224" s="34"/>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C226" s="34"/>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C228" s="34"/>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C230" s="34"/>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C235" s="34"/>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="34"/>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="34"/>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="34"/>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C252" s="34"/>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C254" s="34"/>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C256" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="G12:W12"/>
-    <mergeCell ref="AC3:AO3"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="AL5:AO5"/>
+    <mergeCell ref="Z13:AH15"/>
+    <mergeCell ref="AI13:AV15"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AL9:AO9"/>
+    <mergeCell ref="AL6:AO6"/>
+    <mergeCell ref="AL10:AO10"/>
+    <mergeCell ref="AI10:AK10"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="AI6:AK6"/>
+    <mergeCell ref="AI7:AK7"/>
+    <mergeCell ref="AI8:AK8"/>
+    <mergeCell ref="AI9:AK9"/>
+    <mergeCell ref="AC7:AH7"/>
+    <mergeCell ref="AC6:AH6"/>
+    <mergeCell ref="AC8:AH8"/>
+    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="AL7:AO7"/>
     <mergeCell ref="R11:T11"/>
     <mergeCell ref="U6:W6"/>
@@ -3362,24 +3343,42 @@
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="AI6:AK6"/>
-    <mergeCell ref="AI7:AK7"/>
-    <mergeCell ref="AI8:AK8"/>
-    <mergeCell ref="AI9:AK9"/>
-    <mergeCell ref="AC7:AH7"/>
-    <mergeCell ref="AC6:AH6"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="AC9:AH9"/>
-    <mergeCell ref="AI5:AK5"/>
-    <mergeCell ref="Z13:AH15"/>
-    <mergeCell ref="AI13:AV15"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="AL9:AO9"/>
-    <mergeCell ref="AL6:AO6"/>
-    <mergeCell ref="AL10:AO10"/>
-    <mergeCell ref="AI10:AK10"/>
-    <mergeCell ref="AL5:AO5"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="G12:W12"/>
+    <mergeCell ref="AC3:AO3"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:BD23">
     <cfRule type="expression" dxfId="1" priority="15">
@@ -3398,86 +3397,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B6B2AB-6A6F-45AD-8EE8-E01836CACEB7}">
   <dimension ref="B2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="40.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.88671875" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" customWidth="1"/>
+    <col min="18" max="18" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="100"/>
-    </row>
-    <row r="4" spans="2:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="101"/>
-      <c r="C4" s="102"/>
-      <c r="E4" s="99" t="s">
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="121" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="122"/>
+    </row>
+    <row r="4" spans="2:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="123"/>
+      <c r="C4" s="124"/>
+      <c r="E4" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="100"/>
+      <c r="F4" s="122"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="103" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="104"/>
-      <c r="K4" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="92"/>
-      <c r="N4" s="139" t="s">
-        <v>102</v>
-      </c>
-      <c r="O4" s="136" t="s">
-        <v>85</v>
-      </c>
-      <c r="P4" s="92"/>
-      <c r="R4" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="S4" s="92"/>
-    </row>
-    <row r="5" spans="2:19" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="109"/>
-      <c r="C5" s="110"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+      <c r="H4" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="126"/>
+      <c r="K4" s="109" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="110"/>
+      <c r="N4" s="115" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" s="113" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" s="110"/>
+      <c r="R4" s="109" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="110"/>
+    </row>
+    <row r="5" spans="2:19" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="124"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="106"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="94"/>
-      <c r="N5" s="140"/>
-      <c r="O5" s="137"/>
-      <c r="P5" s="94"/>
-      <c r="R5" s="93"/>
-      <c r="S5" s="94"/>
-    </row>
-    <row r="6" spans="2:19" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="107" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="108"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="128"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="112"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="112"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="112"/>
+    </row>
+    <row r="6" spans="2:19" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="119" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="120"/>
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3485,7 +3484,7 @@
         <v>377.53</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I6" s="20">
         <f>C35*8</f>
@@ -3497,69 +3496,69 @@
       <c r="L6" s="20">
         <v>99</v>
       </c>
-      <c r="N6" s="141">
+      <c r="N6" s="46">
         <v>1</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="P6" s="20">
         <f>N6*(C15+C7+C25)</f>
         <v>648.93999999999994</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="S6" s="20">
         <v>149.99</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="14">
         <v>146.30000000000001</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F7" s="20">
         <f>C28*2</f>
         <v>39.94</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I7" s="20">
         <v>64.88</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L7" s="20">
         <v>19.97</v>
       </c>
-      <c r="N7" s="142">
-        <v>6</v>
+      <c r="N7" s="47">
+        <v>3</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="P7" s="20">
         <f xml:space="preserve"> N7*(Materiales!C16+Materiales!C25+Materiales!C8*2+Materiales!C12)</f>
-        <v>5922.0599999999995</v>
+        <v>2961.0299999999997</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S7" s="20">
-        <v>19.97</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="16">
         <v>141.19</v>
@@ -3572,36 +3571,36 @@
         <v>76.5</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8" s="20">
         <f>14.4*6</f>
         <v>86.4</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L8" s="20">
         <v>25.5</v>
       </c>
-      <c r="N8" s="142">
-        <v>6</v>
+      <c r="N8" s="47">
+        <v>3</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P8" s="20">
         <f xml:space="preserve"> N8*(Materiales!C17+Materiales!C25+Materiales!C8+Materiales!C11)</f>
-        <v>5079.7799999999988</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>49</v>
+        <v>2539.8899999999994</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="S8" s="20">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="E9" s="3" t="s">
@@ -3612,162 +3611,157 @@
         <v>691</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I9" s="20">
         <f>13.53*38</f>
         <v>514.14</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L9" s="20">
         <f>C36</f>
         <v>637</v>
       </c>
-      <c r="N9" s="142">
+      <c r="N9" s="47">
         <v>1</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P9" s="20">
         <f>N9*Materiales!C18</f>
         <v>1558.29</v>
       </c>
-      <c r="R9" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="S9" s="20">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="108"/>
+      <c r="R9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" s="27">
+        <f>SUM(S6:S8)</f>
+        <v>1009.99</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="120"/>
       <c r="E10" s="3" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="F10" s="20">
-        <f>C31*4</f>
-        <v>4008</v>
+        <f>C31*5</f>
+        <v>5010</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I10" s="20">
         <v>400</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L10" s="20">
         <f>10.99*8</f>
         <v>87.92</v>
       </c>
-      <c r="N10" s="142">
+      <c r="N10" s="47">
         <v>2</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P10" s="20">
         <f>N10*Materiales!C19</f>
         <v>3216.6</v>
       </c>
-      <c r="R10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" s="27">
-        <f>SUM(S6:S9)</f>
-        <v>1029.96</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:19" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="14">
         <v>91.8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="F11" s="20">
-        <f>4674*2</f>
-        <v>9348</v>
+        <f>4674</f>
+        <v>4674</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I11" s="20">
         <v>220</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L11" s="27">
         <f>SUM(L6:L10)</f>
         <v>869.39</v>
       </c>
-      <c r="N11" s="142">
+      <c r="N11" s="47">
         <v>2</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P11" s="20">
         <f>N11*(Materiales!C21+Materiales!C25+Materiales!C11+Materiales!C8)</f>
         <v>1571.2599999999998</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R11" s="37"/>
+    </row>
+    <row r="12" spans="2:19" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="18">
         <v>40.99</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="F12" s="20">
-        <f>C33*3</f>
-        <v>9000</v>
+        <f>C33*2</f>
+        <v>6000</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I12" s="20">
         <v>20.99</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
-      <c r="N12" s="142">
-        <v>3</v>
+      <c r="N12" s="47">
+        <v>2</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P12" s="20">
         <f>N12*(Materiales!C21+Materiales!C11+Materiales!C8+Materiales!C25+Materiales!C24)</f>
-        <v>2533.9499999999998</v>
+        <v>1689.3</v>
       </c>
       <c r="R12" s="37"/>
     </row>
-    <row r="13" spans="2:19" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="109"/>
-      <c r="C13" s="110"/>
+    <row r="13" spans="2:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
       <c r="E13" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="20">
         <v>7178</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I13" s="27">
         <f>SUM(I6:I12)</f>
@@ -3775,25 +3769,24 @@
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="N13" s="142">
+      <c r="N13" s="47">
         <v>2</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P13" s="20">
         <f>N13*(Materiales!C20+Materiales!C25+Materiales!C11+Materiales!C8)</f>
         <v>2781.42</v>
       </c>
-      <c r="R13" s="37"/>
-    </row>
-    <row r="14" spans="2:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="108"/>
+    </row>
+    <row r="14" spans="2:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="120"/>
       <c r="E14" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14" s="20">
         <f>C34*70+C37*25</f>
@@ -3801,11 +3794,11 @@
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="7"/>
-      <c r="N14" s="142">
+      <c r="N14" s="47">
         <v>2</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="P14" s="20">
         <f>N14*(Materiales!C21+Materiales!C25+Materiales!C11+Materiales!C8)</f>
@@ -3813,57 +3806,59 @@
       </c>
       <c r="Q14" s="37"/>
     </row>
-    <row r="15" spans="2:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="14">
         <v>459</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
-        <v>31700.77</v>
-      </c>
-      <c r="H15" s="95" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="96"/>
+        <v>25028.77</v>
+      </c>
+      <c r="H15" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="138"/>
       <c r="K15" s="10"/>
       <c r="L15" s="7"/>
-      <c r="N15" s="142"/>
-      <c r="O15" s="138" t="s">
-        <v>86</v>
+      <c r="N15" s="144">
+        <v>2</v>
+      </c>
+      <c r="O15" s="45" t="s">
+        <v>101</v>
       </c>
       <c r="P15" s="20">
-        <f>2*309.99</f>
+        <f>N15*309.99</f>
         <v>619.98</v>
       </c>
       <c r="Q15" s="37"/>
     </row>
-    <row r="16" spans="2:19" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="20">
         <v>620</v>
       </c>
-      <c r="H16" s="97"/>
-      <c r="I16" s="98"/>
-      <c r="N16" s="12"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="140"/>
+      <c r="N16" s="143"/>
       <c r="O16" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P16" s="27">
         <f>SUM(P6:P15)</f>
-        <v>25503.539999999994</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19157.969999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="20">
         <v>570</v>
@@ -3877,9 +3872,9 @@
         <v>910</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="20">
         <v>1558.29</v>
@@ -3888,168 +3883,172 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" s="20">
         <v>1608.3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="20">
         <v>1114.08</v>
       </c>
-      <c r="H20" s="111" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="112"/>
-      <c r="J20" s="87">
-        <f>SUM(F15,I13,I17,L11,P16,S10)</f>
-        <v>62040.069999999992</v>
-      </c>
-      <c r="K20" s="88"/>
-    </row>
-    <row r="21" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="129" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="130"/>
+      <c r="J20" s="133">
+        <f>SUM(F15,I13,I17,L11,P16,S9)</f>
+        <v>49002.529999999992</v>
+      </c>
+      <c r="K20" s="134"/>
+    </row>
+    <row r="21" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="16">
         <v>509</v>
       </c>
-      <c r="H21" s="113"/>
-      <c r="I21" s="114"/>
-      <c r="J21" s="89"/>
-      <c r="K21" s="90"/>
-    </row>
-    <row r="22" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="109"/>
-      <c r="C22" s="110"/>
-    </row>
-    <row r="23" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="107" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="108"/>
-    </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21" s="131"/>
+      <c r="I21" s="132"/>
+      <c r="J21" s="135"/>
+      <c r="K21" s="136"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+    </row>
+    <row r="23" spans="2:12" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="120"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C24" s="14">
         <v>59.02</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="16">
         <v>43.64</v>
       </c>
-      <c r="K25" s="135"/>
-      <c r="L25" s="135"/>
-    </row>
-    <row r="26" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="109"/>
-      <c r="C26" s="110"/>
-      <c r="K26" s="135"/>
-    </row>
-    <row r="27" spans="2:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="108"/>
-    </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="K26" s="44"/>
+    </row>
+    <row r="27" spans="2:12" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="119" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="120"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" s="20">
         <v>19.97</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C29" s="20">
         <v>25.5</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C30" s="20">
         <v>345.5</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C31" s="20">
         <v>1002</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C32" s="20">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C33" s="20">
         <v>3000</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C34" s="20">
         <v>10.99</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="115" t="s">
-        <v>92</v>
+    <row r="35" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="38" t="s">
+        <v>87</v>
       </c>
       <c r="C35" s="20">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="115" t="s">
-        <v>93</v>
+    <row r="36" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="38" t="s">
+        <v>88</v>
       </c>
       <c r="C36" s="20">
         <v>637</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C37" s="28">
         <v>8.5</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="109"/>
-      <c r="C38" s="110"/>
+    <row r="38" spans="2:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J20:K21"/>
+    <mergeCell ref="K4:L5"/>
+    <mergeCell ref="H15:I16"/>
     <mergeCell ref="R4:S5"/>
     <mergeCell ref="O4:P5"/>
     <mergeCell ref="N4:N5"/>
@@ -4066,10 +4065,6 @@
     <mergeCell ref="H20:I21"/>
     <mergeCell ref="E4:F5"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="K4:L5"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" display="https://www.dell.com/es-es/work/shop/accessories/apd/210-APWV" xr:uid="{A7CA1EDC-A29D-41BB-84C7-1EC45A4421FB}"/>
@@ -4112,7 +4107,7 @@
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4133,79 +4128,79 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="127" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="128"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="127" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="128"/>
-    </row>
-    <row r="3" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-    </row>
-    <row r="4" spans="3:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="141" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="142"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="141" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="142"/>
+    </row>
+    <row r="3" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="3:7" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D4" s="30">
         <v>2300</v>
       </c>
-      <c r="F4" s="107" t="s">
+      <c r="F4" s="119" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="120"/>
+    </row>
+    <row r="5" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="G4" s="108"/>
-    </row>
-    <row r="5" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="D5" s="28">
         <v>150</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G5" s="14">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="F6" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G6" s="20">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F7" s="32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G7" s="20">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F8" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G8" s="16">
         <v>23</v>

</xml_diff>